<commit_message>
added information to tables
</commit_message>
<xml_diff>
--- a/prototüüp.xlsx
+++ b/prototüüp.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -1167,17 +1167,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B99" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>

</xml_diff>